<commit_message>
feat: atualizar script de seed para incluir verificação do curso de Engenharia de Software
</commit_message>
<xml_diff>
--- a/templates/planilha_modelo_provas.xlsx
+++ b/templates/planilha_modelo_provas.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29518"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70EF8587-89ED-42B4-A890-34718E6ED2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE308FDF-9C19-4D49-9D05-94636EE8CF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Provas" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>disciplina</t>
-  </si>
-  <si>
-    <t>professor</t>
   </si>
   <si>
     <t>data</t>
@@ -177,7 +174,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -220,14 +217,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="165" formatCode="h:mm;@"/>
+      <numFmt numFmtId="164" formatCode="h:mm;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -246,11 +243,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7FBFA4D4-FA10-4446-9ED0-CAC3A1A57E1A}" name="Tabela1" displayName="Tabela1" ref="A1:I2" totalsRowShown="0">
-  <autoFilter ref="A1:I2" xr:uid="{7FBFA4D4-FA10-4446-9ED0-CAC3A1A57E1A}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7FBFA4D4-FA10-4446-9ED0-CAC3A1A57E1A}" name="Tabela1" displayName="Tabela1" ref="A1:H2" totalsRowShown="0">
+  <autoFilter ref="A1:H2" xr:uid="{7FBFA4D4-FA10-4446-9ED0-CAC3A1A57E1A}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F1096880-FE2F-4A6E-B284-7A50C136B746}" name="disciplina"/>
-    <tableColumn id="2" xr3:uid="{7E8EC5E4-4A40-43A8-9598-DB3C9B3723CE}" name="professor"/>
     <tableColumn id="3" xr3:uid="{A3A52271-FD83-4F90-A897-42A0778E2B13}" name="data" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{0E564D45-3ABC-4E21-BC3A-9E336D993487}" name="horario" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{D70A5F52-A27D-4A8F-BF11-9FA594F47343}" name="sala"/>
@@ -551,7 +547,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -566,13 +562,13 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -587,9 +583,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2"/>
     </row>
     <row r="3" spans="1:11">
       <c r="K3" s="1"/>
@@ -606,25 +604,25 @@
           <x14:formula1>
             <xm:f>'Lista dias da semana'!$A$1:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F1048576</xm:sqref>
+          <xm:sqref>F3:F1048576 E1:E2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{07BA342F-0748-4120-8A8B-76D6D09B85F4}">
           <x14:formula1>
             <xm:f>'Lista turnos'!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G1048576</xm:sqref>
+          <xm:sqref>G3:G1048576 F1:F2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ACF16365-4DC5-4161-B785-2D88B311FC51}">
           <x14:formula1>
             <xm:f>'Lista cursos'!$A$1:$A$23</xm:f>
           </x14:formula1>
-          <xm:sqref>I1:I1048576</xm:sqref>
+          <xm:sqref>I3:I1048576 H1:H2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{742D291B-FB37-4449-A5C5-5B0E5655B8D6}">
           <x14:formula1>
             <xm:f>'Lista ciclos'!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H1048576</xm:sqref>
+          <xm:sqref>H3:H1048576 G1:G2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -645,37 +643,37 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -696,17 +694,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -729,17 +727,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -760,117 +758,117 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>